<commit_message>
Fixed Earnings NO CHECKS
</commit_message>
<xml_diff>
--- a/Project DataSets.xlsx
+++ b/Project DataSets.xlsx
@@ -913,13 +913,13 @@
     <t>15100</t>
   </si>
   <si>
-    <t>57279151414</t>
+    <t>07279151414</t>
   </si>
   <si>
     <t>01514</t>
   </si>
   <si>
-    <t>57207476833</t>
+    <t>07207476833</t>
   </si>
   <si>
     <t>01611</t>
@@ -928,7 +928,7 @@
     <t>16100</t>
   </si>
   <si>
-    <t>57274569556</t>
+    <t>07274569556</t>
   </si>
   <si>
     <t>02202</t>
@@ -10900,7 +10900,7 @@
         <v>70009.0</v>
       </c>
       <c r="C310" s="41" t="s">
-        <v>358</v>
+        <v>289</v>
       </c>
       <c r="D310" s="46">
         <v>43642.0</v>

</xml_diff>